<commit_message>
pairwise tests, tidy & clean up code
</commit_message>
<xml_diff>
--- a/data/tc2c-outputs/GSEA/GSEA-Adj-Pvals.xlsx
+++ b/data/tc2c-outputs/GSEA/GSEA-Adj-Pvals.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="27">
   <si>
     <t>Factor</t>
   </si>
@@ -31,55 +31,46 @@
     <t>Adj. P-value</t>
   </si>
   <si>
-    <t>Factor 2</t>
+    <t>Factor.2</t>
   </si>
   <si>
-    <t>Factor 3</t>
+    <t>Factor.3</t>
   </si>
   <si>
-    <t>Factor 4</t>
+    <t>Factor.4</t>
   </si>
   <si>
-    <t>Factor 5</t>
+    <t>Factor.5</t>
   </si>
   <si>
-    <t>Factor 6</t>
+    <t>Factor.6</t>
   </si>
   <si>
-    <t>Factor 7</t>
+    <t>Factor.7</t>
   </si>
   <si>
-    <t>Factor 8</t>
+    <t>Factor.8</t>
   </si>
   <si>
-    <t>Factor 9</t>
+    <t>Factor.9</t>
   </si>
   <si>
-    <t>Factor 10</t>
-  </si>
-  <si>
-    <t>Factor 11</t>
-  </si>
-  <si>
-    <t>Factor 12</t>
+    <t>Factor.10</t>
   </si>
   <si>
     <t>ANTIGEN PROCESSING AND PRESENTATION</t>
   </si>
   <si>
-    <t>INTESTINAL IMMUNE NETWORK FOR IGA PRODUCTION</t>
+    <t>NATURAL KILLER CELL MEDIATED CYTOTOXICITY</t>
   </si>
   <si>
-    <t>NATURAL KILLER CELL MEDIATED CYTOTOXICITY</t>
+    <t>CELL ADHESION MOLECULES CAMS</t>
   </si>
   <si>
     <t>CHEMOKINE SIGNALING PATHWAY</t>
   </si>
   <si>
-    <t>AXON GUIDANCE</t>
-  </si>
-  <si>
-    <t>CYTOKINE CYTOKINE RECEPTOR INTERACTION</t>
+    <t>INTESTINAL IMMUNE NETWORK FOR IGA PRODUCTION</t>
   </si>
   <si>
     <t>APOPTOSIS</t>
@@ -88,19 +79,22 @@
     <t>PATHWAYS IN CANCER</t>
   </si>
   <si>
+    <t>ECM RECEPTOR INTERACTION</t>
+  </si>
+  <si>
+    <t>CYTOKINE CYTOKINE RECEPTOR INTERACTION</t>
+  </si>
+  <si>
     <t>SMALL CELL LUNG CANCER</t>
   </si>
   <si>
-    <t>ECM RECEPTOR INTERACTION</t>
-  </si>
-  <si>
-    <t>CELL ADHESION MOLECULES CAMS</t>
+    <t>REGULATION OF ACTIN CYTOSKELETON</t>
   </si>
   <si>
     <t>FOCAL ADHESION</t>
   </si>
   <si>
-    <t>REGULATION OF ACTIN CYTOSKELETON</t>
+    <t>AXON GUIDANCE</t>
   </si>
 </sst>
 </file>
@@ -458,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,16 +483,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>1.554817774658157</v>
+        <v>1.63404704367053</v>
       </c>
       <c r="E2">
         <v>0.001</v>
       </c>
       <c r="F2">
-        <v>0.0143143143143143</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -509,16 +503,16 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>1.396167358514424</v>
+        <v>1.226416282781645</v>
       </c>
       <c r="E3">
-        <v>0.0211055276381909</v>
+        <v>0.0842527582748244</v>
       </c>
       <c r="F3">
-        <v>0.1437185929648237</v>
+        <v>0.3768115942028984</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -529,16 +523,16 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4">
-        <v>1.382268687689774</v>
+        <v>1.138232170208162</v>
       </c>
       <c r="E4">
-        <v>0.0200803212851405</v>
+        <v>0.1221221221221221</v>
       </c>
       <c r="F4">
-        <v>0.1435742971887546</v>
+        <v>0.4762762762762762</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -549,16 +543,16 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>1.352335800460651</v>
+        <v>0.9774223647476566</v>
       </c>
       <c r="E5">
-        <v>0.007007007007007</v>
+        <v>0.5645645645645646</v>
       </c>
       <c r="F5">
-        <v>0.0715715715715715</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -569,16 +563,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>1.304409031086441</v>
+        <v>0.9737438639659364</v>
       </c>
       <c r="E6">
-        <v>0.0481444332998996</v>
+        <v>0.5478348439073515</v>
       </c>
       <c r="F6">
-        <v>0.2125458792125456</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -589,16 +583,16 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>1.253930278831303</v>
+        <v>0.9518134163294294</v>
       </c>
       <c r="E7">
-        <v>0.005005005005005</v>
+        <v>0.6056622851365016</v>
       </c>
       <c r="F7">
-        <v>0.05964297630964291</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -609,16 +603,16 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>1.248339490338021</v>
+        <v>0.9274178382353936</v>
       </c>
       <c r="E8">
-        <v>0.1039354187689202</v>
+        <v>0.7077077077077077</v>
       </c>
       <c r="F8">
-        <v>0.3456456949757114</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -629,16 +623,16 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>1.159103857559752</v>
+        <v>0.8914395635752741</v>
       </c>
       <c r="E9">
-        <v>0.1181181181181181</v>
+        <v>0.8678678678678678</v>
       </c>
       <c r="F9">
-        <v>0.3671932802367585</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -649,16 +643,16 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10">
-        <v>1.124231007115856</v>
+        <v>0.8651421034313868</v>
       </c>
       <c r="E10">
-        <v>0.2417251755265797</v>
+        <v>0.928928928928929</v>
       </c>
       <c r="F10">
-        <v>0.5910475234270414</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -669,16 +663,16 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11">
-        <v>1.028539381819359</v>
+        <v>0.8186543760999153</v>
       </c>
       <c r="E11">
-        <v>0.3773773773773773</v>
+        <v>0.8585757271815446</v>
       </c>
       <c r="F11">
-        <v>0.7392460954104788</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -689,16 +683,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>1.027022561411369</v>
+        <v>0.8167060169836952</v>
       </c>
       <c r="E12">
-        <v>0.4184184184184184</v>
+        <v>0.8388721047331319</v>
       </c>
       <c r="F12">
-        <v>0.7872872872872874</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -709,16 +703,16 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13">
-        <v>1.024170000462779</v>
+        <v>0.8100743404335713</v>
       </c>
       <c r="E13">
-        <v>0.4104104104104104</v>
+        <v>0.9509509509509509</v>
       </c>
       <c r="F13">
-        <v>0.7825158491825158</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -729,16 +723,16 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>0.4730971741506364</v>
+        <v>0.5609566020187828</v>
       </c>
       <c r="E14">
-        <v>0.997983870967742</v>
+        <v>0.997997997997998</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -749,16 +743,16 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D15">
-        <v>1.22720512872655</v>
+        <v>1.547646299580523</v>
       </c>
       <c r="E15">
-        <v>0.07114228456913819</v>
+        <v>0.001</v>
       </c>
       <c r="F15">
-        <v>0.2825929637051878</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -769,16 +763,16 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D16">
-        <v>1.201570497585874</v>
+        <v>1.371138623160387</v>
       </c>
       <c r="E16">
-        <v>0.1364092276830491</v>
+        <v>0.004004004004004</v>
       </c>
       <c r="F16">
-        <v>0.4063858241390838</v>
+        <v>0.02927927927927924</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -789,16 +783,16 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D17">
-        <v>1.178453094031837</v>
+        <v>1.358455670414282</v>
       </c>
       <c r="E17">
-        <v>0.02002002002002</v>
+        <v>0.0150300601202404</v>
       </c>
       <c r="F17">
-        <v>0.1435742971887546</v>
+        <v>0.0976953907815626</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -809,16 +803,16 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D18">
-        <v>1.176654615372652</v>
+        <v>1.003804148528182</v>
       </c>
       <c r="E18">
-        <v>0.1485943775100401</v>
+        <v>0.4854854854854855</v>
       </c>
       <c r="F18">
-        <v>0.4249799196787147</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -829,16 +823,16 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D19">
-        <v>1.163499744727145</v>
+        <v>0.9778108513159284</v>
       </c>
       <c r="E19">
-        <v>0.088088088088088</v>
+        <v>0.5480283114256825</v>
       </c>
       <c r="F19">
-        <v>0.307234063331624</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -849,16 +843,16 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D20">
-        <v>1.14759161416304</v>
+        <v>0.8950854524752753</v>
       </c>
       <c r="E20">
-        <v>0.07707707707707701</v>
+        <v>0.8558558558558559</v>
       </c>
       <c r="F20">
-        <v>0.2899566232899564</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -869,16 +863,16 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21">
-        <v>-1.12520325203252</v>
+        <v>0.8739084266416759</v>
       </c>
       <c r="E21">
-        <v>0.1666666666666666</v>
+        <v>0.8268268268268268</v>
       </c>
       <c r="F21">
-        <v>0.4583333333333331</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -889,16 +883,16 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D22">
-        <v>1.094751857822317</v>
+        <v>0.8282853000868193</v>
       </c>
       <c r="E22">
-        <v>0.2432432432432432</v>
+        <v>0.8488488488488488</v>
       </c>
       <c r="F22">
-        <v>0.5910475234270414</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -909,16 +903,16 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D23">
-        <v>1.069259302402758</v>
+        <v>0.7704775388695898</v>
       </c>
       <c r="E23">
-        <v>0.3093093093093093</v>
+        <v>0.9819819819819821</v>
       </c>
       <c r="F23">
-        <v>0.6504592828122239</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -929,16 +923,16 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D24">
-        <v>0.8895892344783617</v>
+        <v>0.7551038608981676</v>
       </c>
       <c r="E24">
-        <v>0.7327327327327328</v>
+        <v>0.9023162134944612</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -949,16 +943,16 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>0.8670003974368545</v>
+        <v>0.7497689026844858</v>
       </c>
       <c r="E25">
-        <v>0.915915915915916</v>
+        <v>0.9035175879396984</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -969,16 +963,16 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D26">
-        <v>0.7942807724564045</v>
+        <v>0.6933295028202574</v>
       </c>
       <c r="E26">
-        <v>0.958958958958959</v>
+        <v>0.990990990990991</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -989,16 +983,16 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D27">
-        <v>0.4736521095960155</v>
+        <v>0.5247425670287847</v>
       </c>
       <c r="E27">
-        <v>0.998998998998999</v>
+        <v>0.995987963891675</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1009,16 +1003,16 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D28">
-        <v>1.770571114166366</v>
+        <v>1.615411411905057</v>
       </c>
       <c r="E28">
         <v>0.001</v>
       </c>
       <c r="F28">
-        <v>0.0143143143143143</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1029,16 +1023,16 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D29">
-        <v>1.694610503479077</v>
+        <v>1.548254731945439</v>
       </c>
       <c r="E29">
         <v>0.001</v>
       </c>
       <c r="F29">
-        <v>0.0143143143143143</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1049,16 +1043,16 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D30">
-        <v>1.143915562097078</v>
+        <v>1.332752319207556</v>
       </c>
       <c r="E30">
-        <v>0.1471471471471471</v>
+        <v>0.0503524672708962</v>
       </c>
       <c r="F30">
-        <v>0.4249799196787147</v>
+        <v>0.2655840754321632</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1069,16 +1063,16 @@
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D31">
-        <v>1.11874322846213</v>
+        <v>1.311352869748486</v>
       </c>
       <c r="E31">
-        <v>0.2542542542542542</v>
+        <v>0.0431293881644934</v>
       </c>
       <c r="F31">
-        <v>0.5960045990227076</v>
+        <v>0.2402923054878918</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1089,16 +1083,16 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D32">
-        <v>1.085506518471741</v>
+        <v>1.245601191138209</v>
       </c>
       <c r="E32">
-        <v>0.2622622622622622</v>
+        <v>0.009009009009009</v>
       </c>
       <c r="F32">
-        <v>0.5960045990227076</v>
+        <v>0.06200317965023841</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1109,16 +1103,16 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>1.064026836366362</v>
+        <v>1.169975852955091</v>
       </c>
       <c r="E33">
-        <v>0.2882882882882883</v>
+        <v>0.1041041041041041</v>
       </c>
       <c r="F33">
-        <v>0.6258776328986961</v>
+        <v>0.4280832556694625</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1129,16 +1123,16 @@
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D34">
-        <v>1.031963135050052</v>
+        <v>1.01607673144502</v>
       </c>
       <c r="E34">
-        <v>0.4545454545454545</v>
+        <v>0.4817813765182186</v>
       </c>
       <c r="F34">
-        <v>0.8053957572029862</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1149,16 +1143,16 @@
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D35">
-        <v>1.016950590978893</v>
+        <v>0.9664548645282064</v>
       </c>
       <c r="E35">
-        <v>0.4659318637274549</v>
+        <v>0.5544354838709677</v>
       </c>
       <c r="F35">
-        <v>0.8053957572029862</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1169,16 +1163,16 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D36">
-        <v>1.013217793404294</v>
+        <v>0.9193293764697176</v>
       </c>
       <c r="E36">
-        <v>0.4594594594594595</v>
+        <v>0.6370070778564206</v>
       </c>
       <c r="F36">
-        <v>0.8053957572029862</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1189,16 +1183,16 @@
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D37">
-        <v>0.9690106340911766</v>
+        <v>0.8988714241377904</v>
       </c>
       <c r="E37">
-        <v>0.5515515515515516</v>
+        <v>0.7987987987987988</v>
       </c>
       <c r="F37">
-        <v>0.8763541319096875</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1209,16 +1203,16 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D38">
-        <v>0.913157087900734</v>
+        <v>0.8269501177959679</v>
       </c>
       <c r="E38">
-        <v>0.8038038038038038</v>
+        <v>0.8928928928928929</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1229,16 +1223,16 @@
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D39">
-        <v>0.8386517659185351</v>
+        <v>0.7697316823010706</v>
       </c>
       <c r="E39">
-        <v>0.7865055387713998</v>
+        <v>0.968968968968969</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1249,16 +1243,16 @@
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D40">
-        <v>0.6970020308964922</v>
+        <v>0.6078008103352895</v>
       </c>
       <c r="E40">
-        <v>0.9435483870967742</v>
+        <v>0.983983983983984</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1269,16 +1263,16 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D41">
-        <v>1.281603461249755</v>
+        <v>1.582387971696602</v>
       </c>
       <c r="E41">
-        <v>0.025025025025025</v>
+        <v>0.001</v>
       </c>
       <c r="F41">
-        <v>0.1486486486486485</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1289,16 +1283,16 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D42">
-        <v>1.233808603607923</v>
+        <v>-1.487730061349693</v>
       </c>
       <c r="E42">
-        <v>0.031031031031031</v>
+        <v>0.001</v>
       </c>
       <c r="F42">
-        <v>0.1530150840495667</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1309,16 +1303,16 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D43">
-        <v>1.135208301574682</v>
+        <v>1.379199798397344</v>
       </c>
       <c r="E43">
-        <v>0.2479919678714859</v>
+        <v>0.001</v>
       </c>
       <c r="F43">
-        <v>0.5910475234270414</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1332,13 +1326,13 @@
         <v>18</v>
       </c>
       <c r="D44">
-        <v>1.125311619161405</v>
+        <v>1.299445385147865</v>
       </c>
       <c r="E44">
-        <v>0.2324649298597194</v>
+        <v>0.0522088353413654</v>
       </c>
       <c r="F44">
-        <v>0.5910475234270414</v>
+        <v>0.2655840754321632</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1349,16 +1343,16 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D45">
-        <v>1.100119743438039</v>
+        <v>1.177876429411219</v>
       </c>
       <c r="E45">
-        <v>0.281563126252505</v>
+        <v>0.08208208208208199</v>
       </c>
       <c r="F45">
-        <v>0.6258776328986961</v>
+        <v>0.3768115942028984</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1369,16 +1363,16 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D46">
-        <v>1.085708166608145</v>
+        <v>0.979186354071704</v>
       </c>
       <c r="E46">
-        <v>0.2945891783567134</v>
+        <v>0.5835835835835835</v>
       </c>
       <c r="F46">
-        <v>0.6287500373882091</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1389,16 +1383,16 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D47">
-        <v>1.023370366741231</v>
+        <v>0.9528095540877514</v>
       </c>
       <c r="E47">
-        <v>0.3963963963963964</v>
+        <v>0.6004016064257028</v>
       </c>
       <c r="F47">
-        <v>0.7660092524957389</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1409,16 +1403,16 @@
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D48">
-        <v>1.01116185237591</v>
+        <v>0.9416690441967888</v>
       </c>
       <c r="E48">
-        <v>0.4591321897073663</v>
+        <v>0.6462925851703407</v>
       </c>
       <c r="F48">
-        <v>0.8053957572029862</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1429,16 +1423,16 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D49">
-        <v>1.010445911903435</v>
+        <v>0.9044071657109428</v>
       </c>
       <c r="E49">
-        <v>0.4554554554554554</v>
+        <v>0.7204408817635271</v>
       </c>
       <c r="F49">
-        <v>0.8053957572029862</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1449,16 +1443,16 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D50">
-        <v>1.004899745187056</v>
+        <v>0.8701131146351447</v>
       </c>
       <c r="E50">
-        <v>0.4964964964964965</v>
+        <v>0.8448448448448449</v>
       </c>
       <c r="F50">
-        <v>0.8201821468298107</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1469,16 +1463,16 @@
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D51">
-        <v>0.9923764049640776</v>
+        <v>0.8423372156766378</v>
       </c>
       <c r="E51">
-        <v>0.5155155155155156</v>
+        <v>0.9509509509509509</v>
       </c>
       <c r="F51">
-        <v>0.8377127127127127</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1489,16 +1483,16 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D52">
-        <v>0.7984520384929669</v>
+        <v>0.8336015034493424</v>
       </c>
       <c r="E52">
-        <v>0.980980980980981</v>
+        <v>0.9409409409409408</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1509,16 +1503,16 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D53">
-        <v>0.4381090978937226</v>
+        <v>0.6576258731303911</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0.9809619238476954</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1529,16 +1523,16 @@
         <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D54">
-        <v>1.571587712425143</v>
+        <v>1.659280669896279</v>
       </c>
       <c r="E54">
         <v>0.001</v>
       </c>
       <c r="F54">
-        <v>0.0143143143143143</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1549,16 +1543,16 @@
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D55">
-        <v>1.347470970376918</v>
+        <v>1.397617980028401</v>
       </c>
       <c r="E55">
-        <v>0.02002002002002</v>
+        <v>0.002002002002002</v>
       </c>
       <c r="F55">
-        <v>0.1435742971887546</v>
+        <v>0.0156156156156156</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1569,16 +1563,16 @@
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D56">
-        <v>1.240029554931395</v>
+        <v>1.134253831069036</v>
       </c>
       <c r="E56">
-        <v>0.1065326633165829</v>
+        <v>0.1061061061061061</v>
       </c>
       <c r="F56">
-        <v>0.3462311557788944</v>
+        <v>0.4280832556694625</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1589,16 +1583,16 @@
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D57">
-        <v>1.212852290362071</v>
+        <v>1.07425506177618</v>
       </c>
       <c r="E57">
-        <v>0.027027027027027</v>
+        <v>0.2742742742742742</v>
       </c>
       <c r="F57">
-        <v>0.1486486486486485</v>
+        <v>0.9168597168597167</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1612,13 +1606,13 @@
         <v>25</v>
       </c>
       <c r="D58">
-        <v>1.140062202485549</v>
+        <v>1.046976992350187</v>
       </c>
       <c r="E58">
-        <v>0.08408408408408399</v>
+        <v>0.3123123123123123</v>
       </c>
       <c r="F58">
-        <v>0.3006006006006002</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1629,16 +1623,16 @@
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D59">
-        <v>1.121038524584927</v>
+        <v>1.035298125985601</v>
       </c>
       <c r="E59">
-        <v>0.1711711711711711</v>
+        <v>0.3943943943943944</v>
       </c>
       <c r="F59">
-        <v>0.4618391976882541</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1649,16 +1643,16 @@
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D60">
-        <v>1.09879011468729</v>
+        <v>1.003869857546196</v>
       </c>
       <c r="E60">
-        <v>0.2888665997993982</v>
+        <v>0.4874874874874875</v>
       </c>
       <c r="F60">
-        <v>0.6258776328986961</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1669,16 +1663,16 @@
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D61">
-        <v>1.039850576814118</v>
+        <v>0.9864713215198602</v>
       </c>
       <c r="E61">
-        <v>0.3733733733733734</v>
+        <v>0.526686807653575</v>
       </c>
       <c r="F61">
-        <v>0.7392460954104788</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1689,16 +1683,16 @@
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D62">
-        <v>1.014985841828544</v>
+        <v>0.9590540523981526</v>
       </c>
       <c r="E62">
-        <v>0.4674674674674675</v>
+        <v>0.6766766766766766</v>
       </c>
       <c r="F62">
-        <v>0.8053957572029862</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1709,16 +1703,16 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D63">
-        <v>0.9090028605011016</v>
+        <v>0.9236230792284782</v>
       </c>
       <c r="E63">
-        <v>0.7487487487487487</v>
+        <v>0.7397397397397397</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1729,16 +1723,16 @@
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D64">
-        <v>0.7522010311175857</v>
+        <v>0.893807193425501</v>
       </c>
       <c r="E64">
-        <v>0.995995995995996</v>
+        <v>0.7386934673366834</v>
       </c>
       <c r="F64">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1749,16 +1743,16 @@
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D65">
-        <v>0.715893563484657</v>
+        <v>0.8832721763909582</v>
       </c>
       <c r="E65">
-        <v>0.9288577154308616</v>
+        <v>0.7833500501504513</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1769,16 +1763,16 @@
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D66">
-        <v>-0.7053388090349076</v>
+        <v>0.7431123932033193</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0.9409409409409408</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1789,16 +1783,16 @@
         <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D67">
-        <v>1.632748613450108</v>
+        <v>1.704757219557903</v>
       </c>
       <c r="E67">
         <v>0.001</v>
       </c>
       <c r="F67">
-        <v>0.0143143143143143</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1809,16 +1803,16 @@
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D68">
-        <v>1.291710579907686</v>
+        <v>1.329872855556781</v>
       </c>
       <c r="E68">
-        <v>0.049049049049049</v>
+        <v>0.0582914572864321</v>
       </c>
       <c r="F68">
-        <v>0.2125458792125456</v>
+        <v>0.2841708542713565</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1829,16 +1823,16 @@
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D69">
-        <v>1.162707676949359</v>
+        <v>1.038065834090318</v>
       </c>
       <c r="E69">
-        <v>0.079079079079079</v>
+        <v>0.4439959636730575</v>
       </c>
       <c r="F69">
-        <v>0.2899566232899564</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1849,16 +1843,16 @@
         <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D70">
-        <v>1.137601915901472</v>
+        <v>1.020306100113844</v>
       </c>
       <c r="E70">
-        <v>0.2625754527162978</v>
+        <v>0.4384384384384384</v>
       </c>
       <c r="F70">
-        <v>0.5960045990227076</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1869,16 +1863,16 @@
         <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D71">
-        <v>1.110635810214823</v>
+        <v>0.989710320561364</v>
       </c>
       <c r="E71">
-        <v>0.1331331331331331</v>
+        <v>0.5315315315315315</v>
       </c>
       <c r="F71">
-        <v>0.4050646391071923</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1889,16 +1883,16 @@
         <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D72">
-        <v>1.093631160393612</v>
+        <v>0.903012478867723</v>
       </c>
       <c r="E72">
-        <v>0.1981981981981982</v>
+        <v>0.7597597597597597</v>
       </c>
       <c r="F72">
-        <v>0.5248581915248582</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1909,16 +1903,16 @@
         <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D73">
-        <v>1.079949972484184</v>
+        <v>0.9017536071212046</v>
       </c>
       <c r="E73">
-        <v>0.3143143143143143</v>
+        <v>0.6783567134268537</v>
       </c>
       <c r="F73">
-        <v>0.6514050282166224</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1929,16 +1923,16 @@
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D74">
-        <v>1.058978448854363</v>
+        <v>0.8991637241867777</v>
       </c>
       <c r="E74">
-        <v>0.3373373373373373</v>
+        <v>0.7237237237237237</v>
       </c>
       <c r="F74">
-        <v>0.689131989131989</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1949,16 +1943,16 @@
         <v>10</v>
       </c>
       <c r="C75" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D75">
-        <v>0.9544966030028144</v>
+        <v>0.8900097992845758</v>
       </c>
       <c r="E75">
-        <v>0.6186186186186187</v>
+        <v>0.7697697697697697</v>
       </c>
       <c r="F75">
-        <v>0.927617790073776</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1969,16 +1963,16 @@
         <v>10</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D76">
-        <v>0.7231925118145296</v>
+        <v>0.8194728629200083</v>
       </c>
       <c r="E76">
-        <v>0.9192734611503532</v>
+        <v>0.8108108108108109</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1989,16 +1983,16 @@
         <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D77">
-        <v>0.7184554327781398</v>
+        <v>0.7634114256788972</v>
       </c>
       <c r="E77">
-        <v>0.988988988988989</v>
+        <v>0.97997997997998</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2009,16 +2003,16 @@
         <v>10</v>
       </c>
       <c r="C78" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D78">
-        <v>0.6296353377028633</v>
+        <v>0.6066374709046851</v>
       </c>
       <c r="E78">
-        <v>0.9666666666666668</v>
+        <v>0.9705583756345176</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2029,16 +2023,16 @@
         <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D79">
-        <v>0.5919148590664763</v>
+        <v>0.5783911203532529</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>0.9827586206896552</v>
       </c>
       <c r="F79">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2049,16 +2043,16 @@
         <v>11</v>
       </c>
       <c r="C80" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D80">
-        <v>1.566835987374235</v>
+        <v>1.428694279501045</v>
       </c>
       <c r="E80">
-        <v>0.001</v>
+        <v>0.001001001001001</v>
       </c>
       <c r="F80">
-        <v>0.0143143143143143</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2069,16 +2063,16 @@
         <v>11</v>
       </c>
       <c r="C81" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D81">
-        <v>1.19214353947211</v>
+        <v>1.284119539818824</v>
       </c>
       <c r="E81">
-        <v>0.039039039039039</v>
+        <v>0.038038038038038</v>
       </c>
       <c r="F81">
-        <v>0.1860860860860859</v>
+        <v>0.234234234234234</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2089,16 +2083,16 @@
         <v>11</v>
       </c>
       <c r="C82" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D82">
-        <v>1.052759716322039</v>
+        <v>1.094843705577221</v>
       </c>
       <c r="E82">
-        <v>0.3723723723723723</v>
+        <v>0.2382382382382382</v>
       </c>
       <c r="F82">
-        <v>0.7392460954104788</v>
+        <v>0.8710585585585583</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2109,16 +2103,16 @@
         <v>11</v>
       </c>
       <c r="C83" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D83">
-        <v>1.01444797665456</v>
+        <v>1.057650334889833</v>
       </c>
       <c r="E83">
-        <v>0.4324324324324324</v>
+        <v>0.3173173173173173</v>
       </c>
       <c r="F83">
-        <v>0.803088803088803</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2129,16 +2123,16 @@
         <v>11</v>
       </c>
       <c r="C84" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D84">
-        <v>0.9676736340094496</v>
+        <v>1.046566190158133</v>
       </c>
       <c r="E84">
-        <v>0.5935935935935935</v>
+        <v>0.3433433433433433</v>
       </c>
       <c r="F84">
-        <v>0.9127299342353106</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2149,16 +2143,16 @@
         <v>11</v>
       </c>
       <c r="C85" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D85">
-        <v>0.9203041011100112</v>
+        <v>0.9607178728759592</v>
       </c>
       <c r="E85">
-        <v>0.6585612968591692</v>
+        <v>0.5997983870967742</v>
       </c>
       <c r="F85">
-        <v>0.9611039611039611</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2169,16 +2163,16 @@
         <v>11</v>
       </c>
       <c r="C86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D86">
-        <v>0.9091678557148056</v>
+        <v>0.9481714939893876</v>
       </c>
       <c r="E86">
-        <v>0.7087087087087087</v>
+        <v>0.6308926780341023</v>
       </c>
       <c r="F86">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2189,16 +2183,16 @@
         <v>11</v>
       </c>
       <c r="C87" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D87">
-        <v>0.9003537124423737</v>
+        <v>0.9168822827336032</v>
       </c>
       <c r="E87">
-        <v>0.7727727727727728</v>
+        <v>0.8288288288288288</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2209,16 +2203,16 @@
         <v>11</v>
       </c>
       <c r="C88" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D88">
-        <v>0.8963479218222044</v>
+        <v>0.9115416315071588</v>
       </c>
       <c r="E88">
-        <v>0.7294589178356713</v>
+        <v>0.7044088176352705</v>
       </c>
       <c r="F88">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2229,16 +2223,16 @@
         <v>11</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D89">
-        <v>0.8814684151209862</v>
+        <v>0.8660655996450833</v>
       </c>
       <c r="E89">
-        <v>0.7321965897693079</v>
+        <v>0.913913913913914</v>
       </c>
       <c r="F89">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2249,16 +2243,16 @@
         <v>11</v>
       </c>
       <c r="C90" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D90">
-        <v>0.7100786608149414</v>
+        <v>0.7934674403976899</v>
       </c>
       <c r="E90">
-        <v>0.9353535353535354</v>
+        <v>0.965965965965966</v>
       </c>
       <c r="F90">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2269,16 +2263,16 @@
         <v>11</v>
       </c>
       <c r="C91" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D91">
-        <v>0.6291571670907478</v>
+        <v>0.7044317291168568</v>
       </c>
       <c r="E91">
-        <v>0.997997997997998</v>
+        <v>0.9425981873111784</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2289,16 +2283,16 @@
         <v>11</v>
       </c>
       <c r="C92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D92">
-        <v>0.5102474982871897</v>
+        <v>0.6906890361375267</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>0.9585858585858584</v>
       </c>
       <c r="F92">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2309,16 +2303,16 @@
         <v>12</v>
       </c>
       <c r="C93" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D93">
-        <v>1.6240036356668</v>
+        <v>1.686798506448025</v>
       </c>
       <c r="E93">
         <v>0.001</v>
       </c>
       <c r="F93">
-        <v>0.0143143143143143</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2329,16 +2323,16 @@
         <v>12</v>
       </c>
       <c r="C94" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D94">
-        <v>1.34899164801186</v>
+        <v>1.596758963881248</v>
       </c>
       <c r="E94">
-        <v>0.002002002002002</v>
+        <v>0.001</v>
       </c>
       <c r="F94">
-        <v>0.02602602602602599</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2349,16 +2343,16 @@
         <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D95">
-        <v>1.336193215777333</v>
+        <v>1.298935564769516</v>
       </c>
       <c r="E95">
-        <v>0.0230460921843687</v>
+        <v>0.0421686746987951</v>
       </c>
       <c r="F95">
-        <v>0.1486486486486485</v>
+        <v>0.2402923054878918</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2369,16 +2363,16 @@
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D96">
-        <v>1.272532229988355</v>
+        <v>1.130381930276384</v>
       </c>
       <c r="E96">
-        <v>0.017017017017017</v>
+        <v>0.2613521695257316</v>
       </c>
       <c r="F96">
-        <v>0.1435742971887546</v>
+        <v>0.8993589363091351</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2389,16 +2383,16 @@
         <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D97">
-        <v>1.254094974572286</v>
+        <v>0.9833192050397712</v>
       </c>
       <c r="E97">
-        <v>0.013013013013013</v>
+        <v>0.5331325301204819</v>
       </c>
       <c r="F97">
-        <v>0.1240573907240573</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2409,16 +2403,16 @@
         <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D98">
-        <v>1.222596183154215</v>
+        <v>0.898097798559446</v>
       </c>
       <c r="E98">
-        <v>0.1033099297893681</v>
+        <v>0.7757757757757757</v>
       </c>
       <c r="F98">
-        <v>0.3456456949757114</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2432,13 +2426,13 @@
         <v>25</v>
       </c>
       <c r="D99">
-        <v>1.20066917117382</v>
+        <v>0.8965393302197525</v>
       </c>
       <c r="E99">
-        <v>0.027027027027027</v>
+        <v>0.8008008008008008</v>
       </c>
       <c r="F99">
-        <v>0.1486486486486485</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2449,16 +2443,16 @@
         <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D100">
-        <v>-1.056980056980057</v>
+        <v>0.8832340928096134</v>
       </c>
       <c r="E100">
-        <v>0.6666666666666666</v>
+        <v>0.7059415911379657</v>
       </c>
       <c r="F100">
-        <v>0.9629629629629629</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2469,16 +2463,16 @@
         <v>12</v>
       </c>
       <c r="C101" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D101">
-        <v>1.006060107201555</v>
+        <v>0.8392549878261514</v>
       </c>
       <c r="E101">
-        <v>0.4739478957915831</v>
+        <v>0.943943943943944</v>
       </c>
       <c r="F101">
-        <v>0.8068398702166236</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2489,16 +2483,16 @@
         <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D102">
-        <v>0.9471911192645648</v>
+        <v>0.8187763067172875</v>
       </c>
       <c r="E102">
-        <v>0.6054490413723511</v>
+        <v>0.9629629629629628</v>
       </c>
       <c r="F102">
-        <v>0.9210554565558108</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2509,16 +2503,16 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D103">
-        <v>0.8129114124705596</v>
+        <v>0.8158894727616071</v>
       </c>
       <c r="E103">
-        <v>0.9109109109109108</v>
+        <v>0.8898898898898899</v>
       </c>
       <c r="F103">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2529,16 +2523,16 @@
         <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D104">
-        <v>0.7380654781156629</v>
+        <v>0.8116688371795174</v>
       </c>
       <c r="E104">
-        <v>0.996996996996997</v>
+        <v>0.8296370967741935</v>
       </c>
       <c r="F104">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2549,16 +2543,16 @@
         <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D105">
-        <v>0.7301471540468633</v>
+        <v>0.5407374706960218</v>
       </c>
       <c r="E105">
-        <v>0.9202825428859738</v>
+        <v>0.995991983967936</v>
       </c>
       <c r="F105">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2569,16 +2563,16 @@
         <v>13</v>
       </c>
       <c r="C106" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D106">
-        <v>1.55242360951047</v>
+        <v>1.691094867184779</v>
       </c>
       <c r="E106">
         <v>0.001</v>
       </c>
       <c r="F106">
-        <v>0.0143143143143143</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2589,16 +2583,16 @@
         <v>13</v>
       </c>
       <c r="C107" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D107">
-        <v>1.264876491983844</v>
+        <v>1.639061714775241</v>
       </c>
       <c r="E107">
-        <v>0.0701402805611222</v>
+        <v>0.001</v>
       </c>
       <c r="F107">
-        <v>0.2825929637051878</v>
+        <v>0.008365508365508355</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2609,16 +2603,16 @@
         <v>13</v>
       </c>
       <c r="C108" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D108">
-        <v>1.252404906104229</v>
+        <v>1.265452445304006</v>
       </c>
       <c r="E108">
-        <v>0.019019019019019</v>
+        <v>0.0869565217391304</v>
       </c>
       <c r="F108">
-        <v>0.1435742971887546</v>
+        <v>0.3768115942028984</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2629,16 +2623,16 @@
         <v>13</v>
       </c>
       <c r="C109" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D109">
-        <v>1.235132416879183</v>
+        <v>1.166867493491491</v>
       </c>
       <c r="E109">
-        <v>0.044044044044044</v>
+        <v>0.1913827655310621</v>
       </c>
       <c r="F109">
-        <v>0.203170912848332</v>
+        <v>0.722315598939815</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2649,16 +2643,16 @@
         <v>13</v>
       </c>
       <c r="C110" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D110">
-        <v>1.215134884544392</v>
+        <v>1.071053058630016</v>
       </c>
       <c r="E110">
-        <v>0.031031031031031</v>
+        <v>0.2482482482482482</v>
       </c>
       <c r="F110">
-        <v>0.1530150840495667</v>
+        <v>0.88015288015288</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2669,16 +2663,16 @@
         <v>13</v>
       </c>
       <c r="C111" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D111">
-        <v>0.996720895347282</v>
+        <v>1.052086269198503</v>
       </c>
       <c r="E111">
-        <v>0.4834834834834834</v>
+        <v>0.3780241935483871</v>
       </c>
       <c r="F111">
-        <v>0.8133898604486839</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2689,16 +2683,16 @@
         <v>13</v>
       </c>
       <c r="C112" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D112">
-        <v>0.9965896386649165</v>
+        <v>1.044558544948522</v>
       </c>
       <c r="E112">
-        <v>0.4989919354838709</v>
+        <v>0.3753753753753753</v>
       </c>
       <c r="F112">
-        <v>0.8201821468298107</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2709,16 +2703,16 @@
         <v>13</v>
       </c>
       <c r="C113" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D113">
-        <v>0.8291613562972578</v>
+        <v>1.041324350504294</v>
       </c>
       <c r="E113">
-        <v>0.8253012048192772</v>
+        <v>0.3493493493493493</v>
       </c>
       <c r="F113">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2729,16 +2723,16 @@
         <v>13</v>
       </c>
       <c r="C114" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D114">
-        <v>0.8080552364362742</v>
+        <v>0.939000219786939</v>
       </c>
       <c r="E114">
-        <v>0.96996996996997</v>
+        <v>0.7257257257257257</v>
       </c>
       <c r="F114">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2749,16 +2743,16 @@
         <v>13</v>
       </c>
       <c r="C115" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D115">
-        <v>0.8074362799062064</v>
+        <v>0.9154087354588596</v>
       </c>
       <c r="E115">
-        <v>0.8998998998998999</v>
+        <v>0.6890672016048145</v>
       </c>
       <c r="F115">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2769,16 +2763,16 @@
         <v>13</v>
       </c>
       <c r="C116" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D116">
-        <v>0.7299548409698281</v>
+        <v>0.8241680919849358</v>
       </c>
       <c r="E116">
-        <v>0.9129554655870444</v>
+        <v>0.8798798798798799</v>
       </c>
       <c r="F116">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -2789,16 +2783,16 @@
         <v>13</v>
       </c>
       <c r="C117" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D117">
-        <v>0.6662177165006005</v>
+        <v>0.8036065962059269</v>
       </c>
       <c r="E117">
-        <v>0.9537688442211056</v>
+        <v>0.8514056224899599</v>
       </c>
       <c r="F117">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2809,536 +2803,16 @@
         <v>13</v>
       </c>
       <c r="C118" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D118">
-        <v>0.6186705817227225</v>
+        <v>0.523945139130242</v>
       </c>
       <c r="E118">
-        <v>0.9859578736208626</v>
+        <v>0.997997997997998</v>
       </c>
       <c r="F118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119" s="1">
-        <v>117</v>
-      </c>
-      <c r="B119" t="s">
-        <v>14</v>
-      </c>
-      <c r="C119" t="s">
-        <v>16</v>
-      </c>
-      <c r="D119">
-        <v>1.471046763721301</v>
-      </c>
-      <c r="E119">
-        <v>0.001</v>
-      </c>
-      <c r="F119">
-        <v>0.0143143143143143</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" s="1">
-        <v>118</v>
-      </c>
-      <c r="B120" t="s">
-        <v>14</v>
-      </c>
-      <c r="C120" t="s">
-        <v>18</v>
-      </c>
-      <c r="D120">
-        <v>1.466710882688958</v>
-      </c>
-      <c r="E120">
-        <v>0.001001001001001</v>
-      </c>
-      <c r="F120">
-        <v>0.0143143143143143</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" s="1">
-        <v>119</v>
-      </c>
-      <c r="B121" t="s">
-        <v>14</v>
-      </c>
-      <c r="C121" t="s">
-        <v>20</v>
-      </c>
-      <c r="D121">
-        <v>1.330599228234583</v>
-      </c>
-      <c r="E121">
-        <v>0.027027027027027</v>
-      </c>
-      <c r="F121">
-        <v>0.1486486486486485</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" s="1">
-        <v>120</v>
-      </c>
-      <c r="B122" t="s">
-        <v>14</v>
-      </c>
-      <c r="C122" t="s">
-        <v>19</v>
-      </c>
-      <c r="D122">
-        <v>1.107986574088585</v>
-      </c>
-      <c r="E122">
-        <v>0.2272272272272272</v>
-      </c>
-      <c r="F122">
-        <v>0.5907907907907908</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" s="1">
-        <v>121</v>
-      </c>
-      <c r="B123" t="s">
-        <v>14</v>
-      </c>
-      <c r="C123" t="s">
-        <v>23</v>
-      </c>
-      <c r="D123">
-        <v>1.088410026337045</v>
-      </c>
-      <c r="E123">
-        <v>0.2472472472472472</v>
-      </c>
-      <c r="F123">
-        <v>0.5910475234270414</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="1">
-        <v>122</v>
-      </c>
-      <c r="B124" t="s">
-        <v>14</v>
-      </c>
-      <c r="C124" t="s">
-        <v>21</v>
-      </c>
-      <c r="D124">
-        <v>0.9245085827412196</v>
-      </c>
-      <c r="E124">
-        <v>0.7957957957957958</v>
-      </c>
-      <c r="F124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" s="1">
-        <v>123</v>
-      </c>
-      <c r="B125" t="s">
-        <v>14</v>
-      </c>
-      <c r="C125" t="s">
-        <v>27</v>
-      </c>
-      <c r="D125">
-        <v>0.9062008706436248</v>
-      </c>
-      <c r="E125">
-        <v>0.7847847847847848</v>
-      </c>
-      <c r="F125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="1">
-        <v>124</v>
-      </c>
-      <c r="B126" t="s">
-        <v>14</v>
-      </c>
-      <c r="C126" t="s">
-        <v>24</v>
-      </c>
-      <c r="D126">
-        <v>0.8958843499286282</v>
-      </c>
-      <c r="E126">
-        <v>0.7161484453360081</v>
-      </c>
-      <c r="F126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" s="1">
-        <v>125</v>
-      </c>
-      <c r="B127" t="s">
-        <v>14</v>
-      </c>
-      <c r="C127" t="s">
-        <v>25</v>
-      </c>
-      <c r="D127">
-        <v>0.8771640512933182</v>
-      </c>
-      <c r="E127">
-        <v>0.8858858858858859</v>
-      </c>
-      <c r="F127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" s="1">
-        <v>126</v>
-      </c>
-      <c r="B128" t="s">
-        <v>14</v>
-      </c>
-      <c r="C128" t="s">
-        <v>17</v>
-      </c>
-      <c r="D128">
-        <v>0.8629078286070003</v>
-      </c>
-      <c r="E128">
-        <v>0.7673716012084593</v>
-      </c>
-      <c r="F128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129" s="1">
-        <v>127</v>
-      </c>
-      <c r="B129" t="s">
-        <v>14</v>
-      </c>
-      <c r="C129" t="s">
-        <v>28</v>
-      </c>
-      <c r="D129">
-        <v>0.8306277932832435</v>
-      </c>
-      <c r="E129">
-        <v>0.8036253776435045</v>
-      </c>
-      <c r="F129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130" s="1">
-        <v>128</v>
-      </c>
-      <c r="B130" t="s">
-        <v>14</v>
-      </c>
-      <c r="C130" t="s">
-        <v>22</v>
-      </c>
-      <c r="D130">
-        <v>0.7894506353924783</v>
-      </c>
-      <c r="E130">
-        <v>0.8561368209255533</v>
-      </c>
-      <c r="F130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
-      <c r="A131" s="1">
-        <v>129</v>
-      </c>
-      <c r="B131" t="s">
-        <v>14</v>
-      </c>
-      <c r="C131" t="s">
-        <v>26</v>
-      </c>
-      <c r="D131">
-        <v>0.618600649285855</v>
-      </c>
-      <c r="E131">
-        <v>0.998998998998999</v>
-      </c>
-      <c r="F131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
-      <c r="A132" s="1">
-        <v>130</v>
-      </c>
-      <c r="B132" t="s">
-        <v>15</v>
-      </c>
-      <c r="C132" t="s">
-        <v>17</v>
-      </c>
-      <c r="D132">
-        <v>1.365407669489976</v>
-      </c>
-      <c r="E132">
-        <v>0.0292633703329969</v>
-      </c>
-      <c r="F132">
-        <v>0.1530150840495667</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
-      <c r="A133" s="1">
-        <v>131</v>
-      </c>
-      <c r="B133" t="s">
-        <v>15</v>
-      </c>
-      <c r="C133" t="s">
-        <v>16</v>
-      </c>
-      <c r="D133">
-        <v>1.352268110720499</v>
-      </c>
-      <c r="E133">
-        <v>0.006006006006006</v>
-      </c>
-      <c r="F133">
-        <v>0.06606606606606599</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" s="1">
-        <v>132</v>
-      </c>
-      <c r="B134" t="s">
-        <v>15</v>
-      </c>
-      <c r="C134" t="s">
-        <v>18</v>
-      </c>
-      <c r="D134">
-        <v>1.254157101128232</v>
-      </c>
-      <c r="E134">
-        <v>0.07429718875502</v>
-      </c>
-      <c r="F134">
-        <v>0.2871485943775097</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
-      <c r="A135" s="1">
-        <v>133</v>
-      </c>
-      <c r="B135" t="s">
-        <v>15</v>
-      </c>
-      <c r="C135" t="s">
-        <v>24</v>
-      </c>
-      <c r="D135">
-        <v>1.19485966184478</v>
-      </c>
-      <c r="E135">
-        <v>0.1601601601601601</v>
-      </c>
-      <c r="F135">
-        <v>0.4490765275078999</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="1">
-        <v>134</v>
-      </c>
-      <c r="B136" t="s">
-        <v>15</v>
-      </c>
-      <c r="C136" t="s">
-        <v>23</v>
-      </c>
-      <c r="D136">
-        <v>1.191813498234548</v>
-      </c>
-      <c r="E136">
-        <v>0.069069069069069</v>
-      </c>
-      <c r="F136">
-        <v>0.2825929637051878</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6">
-      <c r="A137" s="1">
-        <v>135</v>
-      </c>
-      <c r="B137" t="s">
-        <v>15</v>
-      </c>
-      <c r="C137" t="s">
-        <v>27</v>
-      </c>
-      <c r="D137">
-        <v>1.144221322469306</v>
-      </c>
-      <c r="E137">
-        <v>0.1161161161161161</v>
-      </c>
-      <c r="F137">
-        <v>0.3671932802367585</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
-      <c r="A138" s="1">
-        <v>136</v>
-      </c>
-      <c r="B138" t="s">
-        <v>15</v>
-      </c>
-      <c r="C138" t="s">
-        <v>20</v>
-      </c>
-      <c r="D138">
-        <v>0.9893365398789709</v>
-      </c>
-      <c r="E138">
-        <v>0.5455455455455456</v>
-      </c>
-      <c r="F138">
-        <v>0.8763541319096875</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
-      <c r="A139" s="1">
-        <v>137</v>
-      </c>
-      <c r="B139" t="s">
-        <v>15</v>
-      </c>
-      <c r="C139" t="s">
-        <v>19</v>
-      </c>
-      <c r="D139">
-        <v>0.9808508886003589</v>
-      </c>
-      <c r="E139">
-        <v>0.5685685685685685</v>
-      </c>
-      <c r="F139">
-        <v>0.8934648934648934</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
-      <c r="A140" s="1">
-        <v>138</v>
-      </c>
-      <c r="B140" t="s">
-        <v>15</v>
-      </c>
-      <c r="C140" t="s">
-        <v>25</v>
-      </c>
-      <c r="D140">
-        <v>0.9624050986862894</v>
-      </c>
-      <c r="E140">
-        <v>0.6586586586586587</v>
-      </c>
-      <c r="F140">
-        <v>0.9611039611039611</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="A141" s="1">
-        <v>139</v>
-      </c>
-      <c r="B141" t="s">
-        <v>15</v>
-      </c>
-      <c r="C141" t="s">
-        <v>28</v>
-      </c>
-      <c r="D141">
-        <v>0.9566969357144932</v>
-      </c>
-      <c r="E141">
-        <v>0.5933400605449042</v>
-      </c>
-      <c r="F141">
-        <v>0.9127299342353106</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="A142" s="1">
-        <v>140</v>
-      </c>
-      <c r="B142" t="s">
-        <v>15</v>
-      </c>
-      <c r="C142" t="s">
-        <v>22</v>
-      </c>
-      <c r="D142">
-        <v>0.9344688069551164</v>
-      </c>
-      <c r="E142">
-        <v>0.6227364185110664</v>
-      </c>
-      <c r="F142">
-        <v>0.927617790073776</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
-      <c r="A143" s="1">
-        <v>141</v>
-      </c>
-      <c r="B143" t="s">
-        <v>15</v>
-      </c>
-      <c r="C143" t="s">
-        <v>21</v>
-      </c>
-      <c r="D143">
-        <v>0.8905990461032972</v>
-      </c>
-      <c r="E143">
-        <v>0.8358358358358359</v>
-      </c>
-      <c r="F143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
-      <c r="A144" s="1">
-        <v>142</v>
-      </c>
-      <c r="B144" t="s">
-        <v>15</v>
-      </c>
-      <c r="C144" t="s">
-        <v>26</v>
-      </c>
-      <c r="D144">
-        <v>0.6941237604894652</v>
-      </c>
-      <c r="E144">
-        <v>0.996996996996997</v>
-      </c>
-      <c r="F144">
-        <v>1</v>
+        <v>0.997997997997998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>